<commit_message>
venn diagram of databases, charts of titles per year
</commit_message>
<xml_diff>
--- a/data/artisanal-spreadsheets/CSmith-in-ESTC-ECCO-TCP-Hathi.xlsx
+++ b/data/artisanal-spreadsheets/CSmith-in-ESTC-ECCO-TCP-Hathi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrence/Desktop/desktop/THE-DISS/data/artisanal-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{114EAA24-B4DB-E44F-B82E-CDC672546853}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0285E2D-1505-F147-8494-C21DA724BEAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16820" xr2:uid="{F1CEE9FA-3E7A-E946-882F-C50E19AAEEF5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="55">
   <si>
     <t>year</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>Natural History of Birds</t>
+  </si>
+  <si>
+    <t>Gutenberg</t>
+  </si>
+  <si>
+    <t>Gutenberg yes</t>
+  </si>
+  <si>
+    <t>Gutenberg no</t>
+  </si>
+  <si>
+    <t>Works printedin England, 1784-1807</t>
   </si>
 </sst>
 </file>
@@ -551,15 +563,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7209A4B9-770B-374E-BAA2-5F2F8B8B9F15}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H48"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="59" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,8 +596,11 @@
       <c r="H1" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1784</v>
       </c>
@@ -596,7 +611,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>36</v>
@@ -610,8 +625,11 @@
       <c r="H2" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1784</v>
       </c>
@@ -636,8 +654,11 @@
       <c r="H3" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1786</v>
       </c>
@@ -662,8 +683,11 @@
       <c r="H4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1787</v>
       </c>
@@ -688,8 +712,11 @@
       <c r="H5" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>1788</v>
       </c>
@@ -714,8 +741,11 @@
       <c r="H6" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1788</v>
       </c>
@@ -740,8 +770,11 @@
       <c r="H7" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I7" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1789</v>
       </c>
@@ -766,8 +799,11 @@
       <c r="H8" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1789</v>
       </c>
@@ -792,8 +828,11 @@
       <c r="H9" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I9" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1789</v>
       </c>
@@ -818,8 +857,11 @@
       <c r="H10" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I10" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1790</v>
       </c>
@@ -844,8 +886,11 @@
       <c r="H11" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>1791</v>
       </c>
@@ -870,8 +915,11 @@
       <c r="H12" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>1791</v>
       </c>
@@ -896,8 +944,11 @@
       <c r="H13" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I13" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>1792</v>
       </c>
@@ -922,8 +973,11 @@
       <c r="H14" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I14" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>1792</v>
       </c>
@@ -948,8 +1002,11 @@
       <c r="H15" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I15" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>1792</v>
       </c>
@@ -974,8 +1031,11 @@
       <c r="H16" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I16" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1793</v>
       </c>
@@ -1000,8 +1060,11 @@
       <c r="H17" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>1793</v>
       </c>
@@ -1026,8 +1089,11 @@
       <c r="H18" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>1793</v>
       </c>
@@ -1052,8 +1118,11 @@
       <c r="H19" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>1794</v>
       </c>
@@ -1078,8 +1147,11 @@
       <c r="H20" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>1794</v>
       </c>
@@ -1104,8 +1176,11 @@
       <c r="H21" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>1795</v>
       </c>
@@ -1130,8 +1205,11 @@
       <c r="H22" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>1795</v>
       </c>
@@ -1156,8 +1234,11 @@
       <c r="H23" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>1795</v>
       </c>
@@ -1182,8 +1263,11 @@
       <c r="H24" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>1795</v>
       </c>
@@ -1208,8 +1292,11 @@
       <c r="H25" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>1795</v>
       </c>
@@ -1234,8 +1321,11 @@
       <c r="H26" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1796</v>
       </c>
@@ -1260,8 +1350,11 @@
       <c r="H27" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>1796</v>
       </c>
@@ -1286,8 +1379,11 @@
       <c r="H28" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>1796</v>
       </c>
@@ -1312,8 +1408,11 @@
       <c r="H29" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>1797</v>
       </c>
@@ -1338,8 +1437,11 @@
       <c r="H30" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>1797</v>
       </c>
@@ -1364,8 +1466,11 @@
       <c r="H31" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I31" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1798</v>
       </c>
@@ -1390,8 +1495,11 @@
       <c r="H32" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I32" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>1798</v>
       </c>
@@ -1416,8 +1524,11 @@
       <c r="H33" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I33" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>1798</v>
       </c>
@@ -1442,8 +1553,11 @@
       <c r="H34" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I34" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>1799</v>
       </c>
@@ -1468,8 +1582,11 @@
       <c r="H35" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I35" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>1799</v>
       </c>
@@ -1494,8 +1611,11 @@
       <c r="H36" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I36" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>1799</v>
       </c>
@@ -1520,8 +1640,11 @@
       <c r="H37" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I37" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>1800</v>
       </c>
@@ -1546,8 +1669,11 @@
       <c r="H38" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>1800</v>
       </c>
@@ -1572,8 +1698,11 @@
       <c r="H39" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I39" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>1800</v>
       </c>
@@ -1598,8 +1727,11 @@
       <c r="H40" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I40" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>1800</v>
       </c>
@@ -1624,8 +1756,11 @@
       <c r="H41" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I41" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>1800</v>
       </c>
@@ -1650,8 +1785,11 @@
       <c r="H42" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I42" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>1800</v>
       </c>
@@ -1676,8 +1814,11 @@
       <c r="H43" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I43" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>1802</v>
       </c>
@@ -1702,8 +1843,11 @@
       <c r="H44" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I44" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>1804</v>
       </c>
@@ -1728,8 +1872,11 @@
       <c r="H45" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I45" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>1806</v>
       </c>
@@ -1752,8 +1899,11 @@
       <c r="H46" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I46" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>1807</v>
       </c>
@@ -1778,8 +1928,11 @@
       <c r="H47" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I47" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>1807</v>
       </c>
@@ -1803,6 +1956,9 @@
       </c>
       <c r="H48" s="2" t="s">
         <v>44</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>